<commit_message>
20200622 update pig snps list
</commit_message>
<xml_diff>
--- a/data/20200622_pigmentation_snps.xlsx
+++ b/data/20200622_pigmentation_snps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettell/Documents/Repositories/racist_hypothesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C91582-25B8-6143-AE6F-11918B22EE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761EBE6F-880D-CA41-9CB6-C4F83F9960EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30480" yWindow="3140" windowWidth="26440" windowHeight="15040" activeTab="2" xr2:uid="{19E29DA2-5961-024B-9A89-C7CEE8427B6F}"/>
+    <workbookView xWindow="30480" yWindow="3140" windowWidth="26440" windowHeight="15040" activeTab="5" xr2:uid="{19E29DA2-5961-024B-9A89-C7CEE8427B6F}"/>
   </bookViews>
   <sheets>
     <sheet name="20190321_Jonnalagadda-et-al" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="20150512_Liu-et-al" sheetId="5" r:id="rId3"/>
     <sheet name="20121031_Candille-et-al" sheetId="3" r:id="rId4"/>
     <sheet name="20100614_Gerstenblith-et-al" sheetId="2" r:id="rId5"/>
+    <sheet name="20080516_Han-et-al" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
   <si>
     <t>rs3002288</t>
   </si>
@@ -316,6 +317,39 @@
   </si>
   <si>
     <t>rs6059655</t>
+  </si>
+  <si>
+    <t>rs6497268</t>
+  </si>
+  <si>
+    <t>rs4904866</t>
+  </si>
+  <si>
+    <t>rs8033165</t>
+  </si>
+  <si>
+    <t>rs35391</t>
+  </si>
+  <si>
+    <t>rs8007923</t>
+  </si>
+  <si>
+    <t>rs10861741</t>
+  </si>
+  <si>
+    <t>rs9806558</t>
+  </si>
+  <si>
+    <t>rs9392056</t>
+  </si>
+  <si>
+    <t>rs2493040</t>
+  </si>
+  <si>
+    <t>rs12142165</t>
+  </si>
+  <si>
+    <t>rs16950987</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B728D1D5-83A9-A143-905C-813B4B22C98B}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1395,4 +1429,214 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64239EBE-8879-5F4F-A869-32CAA425CB44}">
+  <dimension ref="A1:A39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>